<commit_message>
updates to visualizations mostly
</commit_message>
<xml_diff>
--- a/Models' Performance.xlsx
+++ b/Models' Performance.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eaber\Documents\9. Model Engineering - DLMDSME01\DLMDSME01_Credit_Routing_Solution\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eaber\Documents\9. Model Engineering - DLMDSME01\DLMDSME01_CreditCard_Routing_Solution\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C10F38E3-916B-42C4-B7AA-95B62CD62951}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E6CD9E6-8F79-4A05-B34C-7148E7DC9088}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{EF8721B7-6589-4713-A122-1BB5CA67F8BA}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{EF8721B7-6589-4713-A122-1BB5CA67F8BA}"/>
   </bookViews>
   <sheets>
     <sheet name="AUC" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="14">
   <si>
     <t>LR</t>
   </si>
@@ -71,12 +71,6 @@
   </si>
   <si>
     <t>DTEDRF</t>
-  </si>
-  <si>
-    <t>DTIDRFDO</t>
-  </si>
-  <si>
-    <t>DTEDRFDO</t>
   </si>
   <si>
     <t>Model</t>
@@ -465,10 +459,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F80F6413-1FC2-489E-B758-7B007D807DCD}">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1:G1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -477,13 +471,11 @@
     <col min="2" max="3" width="8.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>8</v>
@@ -497,16 +489,10 @@
       <c r="E1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G1" s="2" t="s">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>15</v>
       </c>
       <c r="B2" s="4">
         <v>0.62407000000000001</v>
@@ -520,14 +506,8 @@
       <c r="E2" s="4">
         <v>0.62407000000000001</v>
       </c>
-      <c r="F2" s="4">
-        <v>0.62407000000000001</v>
-      </c>
-      <c r="G2" s="4">
-        <v>0.62407000000000001</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
@@ -543,14 +523,8 @@
       <c r="E3" s="4">
         <v>0.62770000000000004</v>
       </c>
-      <c r="F3" s="4">
-        <v>0.62478</v>
-      </c>
-      <c r="G3" s="4">
-        <v>0.62770999999999999</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>1</v>
       </c>
@@ -566,14 +540,8 @@
       <c r="E4" s="4">
         <v>0.58081000000000005</v>
       </c>
-      <c r="F4" s="4">
-        <v>0.58667999999999998</v>
-      </c>
-      <c r="G4" s="4">
-        <v>0.58696999999999999</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
@@ -589,14 +557,8 @@
       <c r="E5" s="4">
         <v>0.57379000000000002</v>
       </c>
-      <c r="F5" s="4">
-        <v>0.49560999999999999</v>
-      </c>
-      <c r="G5" s="4">
-        <v>0.51641000000000004</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>3</v>
       </c>
@@ -612,14 +574,8 @@
       <c r="E6" s="4">
         <v>0.57835999999999999</v>
       </c>
-      <c r="F6" s="4">
-        <v>0.57662000000000002</v>
-      </c>
-      <c r="G6" s="4">
-        <v>0.60082000000000002</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>4</v>
       </c>
@@ -635,14 +591,8 @@
       <c r="E7" s="4">
         <v>0.62183999999999995</v>
       </c>
-      <c r="F7" s="4">
-        <v>0.61107999999999996</v>
-      </c>
-      <c r="G7" s="4">
-        <v>0.62148999999999999</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>5</v>
       </c>
@@ -658,14 +608,8 @@
       <c r="E8" s="4">
         <v>0.54369999999999996</v>
       </c>
-      <c r="F8" s="4">
-        <v>0.53613</v>
-      </c>
-      <c r="G8" s="4">
-        <v>0.54915999999999998</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>6</v>
       </c>
@@ -681,14 +625,8 @@
       <c r="E9" s="4">
         <v>0.62378</v>
       </c>
-      <c r="F9" s="4">
-        <v>0.60740000000000005</v>
-      </c>
-      <c r="G9" s="4">
-        <v>0.62414000000000003</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>7</v>
       </c>
@@ -704,16 +642,10 @@
       <c r="E10" s="4">
         <v>0.65781000000000001</v>
       </c>
-      <c r="F10" s="4">
-        <v>0.66479999999999995</v>
-      </c>
-      <c r="G10" s="4">
-        <v>0.65905999999999998</v>
-      </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B2:G2">
-    <cfRule type="colorScale" priority="1">
+  <conditionalFormatting sqref="B2:E2">
+    <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -722,8 +654,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B3:G11">
-    <cfRule type="colorScale" priority="2">
+  <conditionalFormatting sqref="B3:E11">
+    <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -739,10 +671,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E88145C6-B102-43C4-BF9D-557734D98610}">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -751,13 +683,11 @@
     <col min="2" max="2" width="8.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="7.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>8</v>
@@ -771,14 +701,8 @@
       <c r="E1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -794,14 +718,8 @@
       <c r="E2" s="1">
         <v>4.3400000000000001E-2</v>
       </c>
-      <c r="F2" s="1">
-        <v>3.5499999999999997E-2</v>
-      </c>
-      <c r="G2" s="1">
-        <v>4.9799999999999997E-2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -817,14 +735,8 @@
       <c r="E3" s="1">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="F3" s="1">
-        <v>1.5599999999999999E-2</v>
-      </c>
-      <c r="G3" s="1">
-        <v>4.0000000000000001E-3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
@@ -840,14 +752,8 @@
       <c r="E4" s="1">
         <v>22.581900000000001</v>
       </c>
-      <c r="F4" s="1">
-        <v>40.936199999999999</v>
-      </c>
-      <c r="G4" s="1">
-        <v>46.076700000000002</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
@@ -863,14 +769,8 @@
       <c r="E5" s="1">
         <v>244.6601</v>
       </c>
-      <c r="F5" s="1">
-        <v>267.11200000000002</v>
-      </c>
-      <c r="G5" s="1">
-        <v>86.140900000000002</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
@@ -886,14 +786,8 @@
       <c r="E6" s="1">
         <v>1.32E-2</v>
       </c>
-      <c r="F6" s="1">
-        <v>1.8200000000000001E-2</v>
-      </c>
-      <c r="G6" s="1">
-        <v>1.34E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
@@ -909,14 +803,8 @@
       <c r="E7" s="1">
         <v>0.21199999999999999</v>
       </c>
-      <c r="F7" s="1">
-        <v>0.38669999999999999</v>
-      </c>
-      <c r="G7" s="1">
-        <v>0.32419999999999999</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
@@ -932,14 +820,8 @@
       <c r="E8" s="1">
         <v>0.78390000000000004</v>
       </c>
-      <c r="F8" s="1">
-        <v>0.88219999999999998</v>
-      </c>
-      <c r="G8" s="1">
-        <v>0.77510000000000001</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>7</v>
       </c>
@@ -955,16 +837,10 @@
       <c r="E9" s="1">
         <v>0.21590000000000001</v>
       </c>
-      <c r="F9" s="1">
-        <v>0.2462</v>
-      </c>
-      <c r="G9" s="1">
-        <v>0.255</v>
-      </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B2:G9">
-    <cfRule type="colorScale" priority="1">
+  <conditionalFormatting sqref="B2:E9">
+    <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>

</xml_diff>